<commit_message>
Tried to make 404 page
Not successful.
</commit_message>
<xml_diff>
--- a/Documentation/TimeLog_ConnorPeper.xlsx
+++ b/Documentation/TimeLog_ConnorPeper.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pepercr\Documents\Rose-Local\Software Project\AudienceResponse\CTS5_AudienceResponse\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA7A7693-A0FC-41FA-AD08-8E9F14A464A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9D62EDC-526A-4BF9-AB4C-5B3CDE4ABE79}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5892" yWindow="3120" windowWidth="15372" windowHeight="8280" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -78,7 +78,7 @@
     <t>Worked on the Vision document with the rest of the team. Made some demo ER-Diagrams and UML diagrams in spare time. Attended team meetings</t>
   </si>
   <si>
-    <t>Meeting with professor. Met with team to choose SCRUM master and Product Owner.</t>
+    <t>Meeting with professor. Met with team to choose SCRUM master and Product Owner. Meeting with professor for Daily SCRUM (Took longer than expected). Created Frontend-Backend connection.</t>
   </si>
 </sst>
 </file>
@@ -480,8 +480,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D5" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -599,7 +599,7 @@
         <v>44122</v>
       </c>
       <c r="E9" s="12">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="F9" s="12" t="s">
         <v>13</v>

</xml_diff>

<commit_message>
Got connection to a local database
This was hell, good thing I didn't try to explain it all back at the Hochschule.
</commit_message>
<xml_diff>
--- a/Documentation/TimeLog_ConnorPeper.xlsx
+++ b/Documentation/TimeLog_ConnorPeper.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pepercr\Documents\Rose-Local\Software Project\AudienceResponse\CTS5_AudienceResponse\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9D62EDC-526A-4BF9-AB4C-5B3CDE4ABE79}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC10385E-DDB8-4299-A115-FC0686782D94}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7668" yWindow="2148" windowWidth="15372" windowHeight="8280" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t xml:space="preserve">Time Log </t>
   </si>
@@ -79,6 +79,9 @@
   </si>
   <si>
     <t>Meeting with professor. Met with team to choose SCRUM master and Product Owner. Meeting with professor for Daily SCRUM (Took longer than expected). Created Frontend-Backend connection.</t>
+  </si>
+  <si>
+    <t>Updated ER diagram, created relational schema document. Hosted a meeting with Back-end team. We discussed how we would organize the backend server and what classes we would need.</t>
   </si>
 </sst>
 </file>
@@ -480,8 +483,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+    <sheetView tabSelected="1" topLeftCell="D5" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -621,8 +624,12 @@
         <f t="shared" si="1"/>
         <v>44129</v>
       </c>
-      <c r="E10" s="12"/>
-      <c r="F10" s="12"/>
+      <c r="E10" s="12">
+        <v>4</v>
+      </c>
+      <c r="F10" s="12" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="11" spans="1:6" s="10" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="11">

</xml_diff>

<commit_message>
Results from work today
</commit_message>
<xml_diff>
--- a/Documentation/TimeLog_ConnorPeper.xlsx
+++ b/Documentation/TimeLog_ConnorPeper.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pepercr\Documents\Rose-Local\Software Project\AudienceResponse\CTS5_AudienceResponse\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC10385E-DDB8-4299-A115-FC0686782D94}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF5CB2B7-2C67-4E28-9439-2F3A94D733E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="7668" yWindow="2148" windowWidth="15372" windowHeight="8280" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -81,7 +81,7 @@
     <t>Meeting with professor. Met with team to choose SCRUM master and Product Owner. Meeting with professor for Daily SCRUM (Took longer than expected). Created Frontend-Backend connection.</t>
   </si>
   <si>
-    <t>Updated ER diagram, created relational schema document. Hosted a meeting with Back-end team. We discussed how we would organize the backend server and what classes we would need.</t>
+    <t>Updated ER diagram, created relational schema document. Hosted a meeting with Back-end team. We discussed how we would organize the backend server and what classes we would need. Created connection between local database and locally hosted backend. Finished setting up table definitions within Spring Boot. Finished modeling backend architecture.</t>
   </si>
 </sst>
 </file>
@@ -483,7 +483,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D5" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="D4" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Users can join a session too now
</commit_message>
<xml_diff>
--- a/Documentation/TimeLog_ConnorPeper.xlsx
+++ b/Documentation/TimeLog_ConnorPeper.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pepercr\Documents\Rose-Local\Software Project\AudienceResponse\CTS5_AudienceResponse\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F261DEB-982D-463D-BA11-8598D26C24D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2ECA8A00-048D-40A7-A760-BBF2453F27F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1620" yWindow="1080" windowWidth="17472" windowHeight="9876" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -84,7 +84,7 @@
     <t>Updated ER diagram, created relational schema document. Hosted a meeting with Back-end team. We discussed how we would organize the backend server and what classes we would need. Created connection between local database and locally hosted backend. Finished setting up table definitions within Spring Boot. Finished modeling backend architecture.</t>
   </si>
   <si>
-    <t>Task 1-2: Worked on connecting front end to the backend. Added GET, POST requests with pseudo-database implementation.</t>
+    <t>Task 3: Worked on connecting front end to the backend. Added GET, POST requests handling in the backend for session joins and session creations.</t>
   </si>
 </sst>
 </file>
@@ -651,7 +651,7 @@
         <v>44136</v>
       </c>
       <c r="E11" s="12">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="F11" s="12" t="s">
         <v>15</v>

</xml_diff>

<commit_message>
Fixed the joinSession bug, updated reply()
</commit_message>
<xml_diff>
--- a/Documentation/TimeLog_ConnorPeper.xlsx
+++ b/Documentation/TimeLog_ConnorPeper.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25726"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pepercr\Documents\Rose-Local\Software Project\AudienceResponse\CTS5_AudienceResponse\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17460210-FFF0-4F6A-8A59-E57E1A188D17}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C19B713B-E5B6-4067-8930-76F95E00EA69}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3012" yWindow="2472" windowWidth="17472" windowHeight="9876" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -87,7 +87,7 @@
     <t>Task 3: Worked on connecting front end to the backend. Added GET, POST requests handling in the backend for session joins and session creations. Task 4: Created methods and parameters for getting message (Without reply) from the frontend. Task 6: Create a SPROC do handle createSession and joinSession. No validation</t>
   </si>
   <si>
-    <t>Set up the Database server on the server we got from the CS department. Had a development meeting with Luca and Mihai. Task  16: Created the methods necessary to post a message but did not implement the business logic within those methods. Added documentation to methods to better connect to the front-end. Task 6: Wrapped SPROC inside a transaction. No parameters actually needed to be validated since they are all OUT parameters.</t>
+    <t>Set up the Database server on the server we got from the CS department. Had a development meeting with Luca and Mihai. Task  16: Created the methods necessary to post a message but did not implement the business logic within those methods. Added documentation to methods to better connect to the front-end. Task 6: Wrapped SPROC inside a transaction. No parameters actually needed to be validated since they are all OUT parameters. Fixed the bug that had the session ID always be 2 if the session did not exist.</t>
   </si>
 </sst>
 </file>
@@ -492,8 +492,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+    <sheetView tabSelected="1" topLeftCell="C4" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -682,7 +682,7 @@
         <v>44143</v>
       </c>
       <c r="E12" s="12">
-        <v>3.5</v>
+        <v>5</v>
       </c>
       <c r="F12" s="12" t="s">
         <v>16</v>

</xml_diff>